<commit_message>
fix work with duplicate repay
</commit_message>
<xml_diff>
--- a/src/repay.xlsx
+++ b/src/repay.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olega\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olega\PycharmProjects\portfolio_parse\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="155">
   <si>
     <t>RU000A0JS8T1': {'name_paper': 'Обл. Липецкой области, выпуск 34007', 'volume': 1},</t>
   </si>
@@ -394,6 +394,102 @@
   </si>
   <si>
     <t>7 120,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPNN9': {'name_paper': 'АО "ФСК ЕЭС" ПАО, выпуск 01', 'volume': 70000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0006765096': {'name_paper': 'АП  "Нижнекамскнефтехим" (НКНХ) ПАО, выпуск 02', 'volume': 220}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0009092134': {'name_paper': 'АП "Ленэнерго"  ОАО, выпуск 01', 'volume': 120}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0006944147': {'name_paper': 'АП "Татнефть"  ПАО, выпуск 03', 'volume': 22}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0009029524': {'name_paper': 'АП "Сургутнефтегаз" ОАО, выпуск 01', 'volume': 700}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0009046510': {'name_paper': 'АО "Северсталь" ПАО, выпуск 02', 'volume': 12}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0007976965': {'name_paper': 'АП "АНК "Башнефть" ПАО, выпуск 01', 'volume': 10}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JXK40': {'name_paper': 'Обл. "Группа Компаний ПИК" ПАО, серия БО-П01', 'volume': 7}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPPT1': {'name_paper': 'АО "МРСК Урала" ОАО, выпуск 01', 'volume': 20000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0DQZE3': {'name_paper': 'АО "АФК "Система" ПАО, выпуск 05', 'volume': 600}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0007661625': {'name_paper': 'АО "Газпром" ПАО, выпуск 02', 'volume': 100}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPPN4': {'name_paper': 'АО "МРСК Волги" ПАО, выпуск 01', 'volume': 120000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPN96': {'name_paper': 'АО "МРСК Центра и Приволжья" ОАО, выпуск 01', 'volume': 70000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0ZYQY7': {'name_paper': 'Обл. АФК "Система" ПАО, серия 001P-07', 'volume': 10}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0009046452': {'name_paper': 'АО "НЛМК" ПАО, выпуск 01', 'volume': 150}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU0007252813': {'name_paper': 'АО "АЛРОСА" ПАО, выпуск 03', 'volume': 300}, </t>
+  </si>
+  <si>
+    <t>'RU000A0JVW30': {'name_paper': 'ОФЗ 26217-ПД', 'volume': 6},</t>
+  </si>
+  <si>
+    <t>'RU000A0JREQ7': {'name_paper': 'ОФЗ 26205-ПД', 'volume': 6},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'RU0009029557': {'name_paper': 'АП "СБЕРБАНК России" ПАО', 'volume': 80}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPPG8': {'name_paper': 'АО "МРСК Юга" ПАО, выпуск 01', 'volume': 70000}, </t>
+  </si>
+  <si>
+    <t>'RU0009062467': {'name_paper': 'АО "Газпром нефть"  ПАО, выпуск 01', 'volume': 30},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JWU98': {'name_paper': 'Обл. "Группа ЛСР" ПАО, серия 001P-01', 'volume': 2}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JPFP0': {'name_paper': 'АО "Группа ЛСР" ПАО, выпуск 01', 'volume': 2}, </t>
+  </si>
+  <si>
+    <t>'RU0009024277': {'name_paper': 'АО "ЛУКОЙЛ" ПАО, выпуск 01', 'volume': 2},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A100W29': {'name_paper': 'Обл. ЛК "Роделен" ЗАО, серия 001P-02', 'volume': 1}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A101CB6': {'name_paper': 'Обл. "Лизинг-Трейд" ООО, серия 001P-01', 'volume': 5}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A101FT1': {'name_paper': 'Обл. "Ломбард "Мастер" ООО, серия БО-П07', 'volume': 3}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JNGA5': {'name_paper': 'АО "Юнипро" ПАО, выпуск 02', 'volume': 2000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JP5V6': {'name_paper': 'АО Банк ВТБ ПАО, выпуск 04', 'volume': 80000}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0JR4A1': {'name_paper': 'АО "Московская Биржа" ПАО, выпуск 01', 'volume': 20}, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'RU000A0DKVS5': {'name_paper': 'АО "НОВАТЭК" ПАО, выпуск 02', 'volume': 3}, </t>
+  </si>
+  <si>
+    <t>'RU000A0HM5C1': {'name_paper': 'АО "Таттелеком" ПАО, выпуск 02', 'volume': 10000}</t>
   </si>
 </sst>
 </file>
@@ -712,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,6 +869,166 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>